<commit_message>
submitted to collab file
</commit_message>
<xml_diff>
--- a/Renewables - Spreadsheet.xlsx
+++ b/Renewables - Spreadsheet.xlsx
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -64,12 +64,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="E11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">https://sunpower.maxeon.com/int/sites/default/files/2020-09/sp_mst_MAX3-400-390-370_COM_ds_en_a4_mc4_532420.pdf</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t xml:space="preserve">Producing 24 hr</t>
   </si>
@@ -125,6 +139,9 @@
     <t xml:space="preserve">CMP24175SR</t>
   </si>
   <si>
+    <t xml:space="preserve">Max Power Usage</t>
+  </si>
+  <si>
     <t xml:space="preserve">CMP22225S</t>
   </si>
   <si>
@@ -144,6 +161,30 @@
   </si>
   <si>
     <t xml:space="preserve">Covered footprint</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sunpower </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Maxeon 5</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SPR-MAX5-450-COM</t>
   </si>
   <si>
     <t xml:space="preserve">% of day useful</t>
@@ -156,14 +197,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0%"/>
-    <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="168" formatCode="0.00%"/>
+    <numFmt numFmtId="169" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -201,6 +243,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -336,7 +384,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -421,11 +469,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -433,11 +485,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,15 +594,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.85"/>
@@ -614,7 +675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
@@ -631,50 +692,50 @@
         <v>14</v>
       </c>
       <c r="F4" s="19" t="n">
-        <f aca="false">21.65*42.9*B14</f>
+        <f aca="false">21.65*42.9*B15</f>
         <v>0.5992149306</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>0.11</v>
       </c>
       <c r="H4" s="19" t="n">
-        <f aca="false">($B$10/F4)*G4</f>
+        <f aca="false">($B$11/F4)*G4</f>
         <v>219.530536177197</v>
       </c>
       <c r="I4" s="20" t="n">
-        <f aca="false">H4/$B$5</f>
-        <v>0.024092884871147</v>
+        <f aca="false">H4/$B$7</f>
+        <v>0.0344184069587815</v>
       </c>
       <c r="J4" s="1" t="n">
-        <f aca="false">($B$5/G4)*F4</f>
-        <v>49635.9197495749</v>
+        <f aca="false">($B$7/G4)*F4</f>
+        <v>34745.1438247024</v>
       </c>
       <c r="K4" s="20" t="n">
-        <f aca="false">J4/$B$7</f>
-        <v>20.7530149533394</v>
-      </c>
-      <c r="L4" s="20" t="n">
-        <f aca="false">(H4*$B$12)/$B$5</f>
-        <v>0.00803096162371568</v>
+        <f aca="false">J4/$B$8</f>
+        <v>14.5271104673376</v>
+      </c>
+      <c r="L4" s="21" t="n">
+        <f aca="false">(H4*$B$13)/$B$7</f>
+        <v>0.0114728023195938</v>
       </c>
       <c r="M4" s="1" t="n">
-        <f aca="false">($B$5/(G4*$B$12))*F4</f>
-        <v>148907.759248725</v>
+        <f aca="false">($B$7/(G4*$B$13))*F4</f>
+        <v>104235.431474107</v>
       </c>
       <c r="N4" s="20" t="n">
-        <f aca="false">M4/$B$7</f>
-        <v>62.2590448600183</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
+        <f aca="false">M4/$B$8</f>
+        <v>43.5813314020129</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="22" t="n">
+      <c r="B5" s="23" t="n">
         <f aca="false">AVERAGE(13440, 16347.233, 15360, (2*3840+2*750), 16000, (2*1420+1000),  (2*1420+1000), (2*2500+2*880+880), 2*2200, 6300, 4064.064, 4*980, 2*2200, 4*4320, 4*1500+2*5295, 7000, 5300)</f>
         <v>9111.841</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -684,174 +745,239 @@
         <v>17</v>
       </c>
       <c r="F5" s="19" t="n">
-        <f aca="false">36.4*37.6*B14</f>
+        <f aca="false">36.4*37.6*B15</f>
         <v>0.8829917824</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>0.175</v>
       </c>
       <c r="H5" s="19" t="n">
-        <f aca="false">($B$10/F5)*G5</f>
+        <f aca="false">($B$11/F5)*G5</f>
         <v>237.009779333593</v>
       </c>
       <c r="I5" s="20" t="n">
-        <f aca="false">H5/$B$5</f>
-        <v>0.0260111847137799</v>
+        <f aca="false">H5/$B$7</f>
+        <v>0.0371588353053999</v>
       </c>
       <c r="J5" s="1" t="n">
-        <f aca="false">($B$5/G5)*F5</f>
-        <v>45975.3184316309</v>
+        <f aca="false">($B$7/G5)*F5</f>
+        <v>32182.7229021416</v>
       </c>
       <c r="K5" s="20" t="n">
-        <f aca="false">J5/$B$7</f>
-        <v>19.2225000707144</v>
-      </c>
-      <c r="L5" s="20" t="n">
-        <f aca="false">(H5*$B$12)/$B$5</f>
-        <v>0.0086703949045933</v>
+        <f aca="false">J5/$B$8</f>
+        <v>13.4557500495001</v>
+      </c>
+      <c r="L5" s="21" t="n">
+        <f aca="false">(H5*$B$13)/$B$7</f>
+        <v>0.0123862784351333</v>
       </c>
       <c r="M5" s="1" t="n">
-        <f aca="false">($B$5/(G5*$B$12))*F5</f>
-        <v>137925.955294893</v>
+        <f aca="false">($B$7/(G5*$B$13))*F5</f>
+        <v>96548.1687064249</v>
       </c>
       <c r="N5" s="20" t="n">
-        <f aca="false">M5/$B$7</f>
-        <v>57.6675002121433</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">M5/$B$8</f>
+        <v>40.3672501485003</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="25" t="n">
+        <v>0.7</v>
+      </c>
       <c r="D6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="19" t="n">
-        <f aca="false">31.1*56.3*B14</f>
+        <f aca="false">31.1*56.3*B15</f>
         <v>1.1296299988</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>0.225</v>
       </c>
       <c r="H6" s="19" t="n">
-        <f aca="false">($B$10/F6)*G6</f>
+        <f aca="false">($B$11/F6)*G6</f>
         <v>238.194198795918</v>
       </c>
       <c r="I6" s="20" t="n">
-        <f aca="false">H6/$B$5</f>
-        <v>0.0261411715586255</v>
+        <f aca="false">H6/$B$7</f>
+        <v>0.0373445307980365</v>
       </c>
       <c r="J6" s="1" t="n">
-        <f aca="false">($B$5/G6)*F6</f>
-        <v>45746.706390648</v>
+        <f aca="false">($B$7/G6)*F6</f>
+        <v>32022.6944734536</v>
       </c>
       <c r="K6" s="20" t="n">
-        <f aca="false">J6/$B$7</f>
-        <v>19.1269162852428</v>
-      </c>
-      <c r="L6" s="20" t="n">
-        <f aca="false">(H6*$B$12)/$B$5</f>
-        <v>0.00871372385287518</v>
+        <f aca="false">J6/$B$8</f>
+        <v>13.3888413996699</v>
+      </c>
+      <c r="L6" s="21" t="n">
+        <f aca="false">(H6*$B$13)/$B$7</f>
+        <v>0.0124481769326788</v>
       </c>
       <c r="M6" s="1" t="n">
-        <f aca="false">($B$5/(G6*$B$12))*F6</f>
-        <v>137240.119171944</v>
+        <f aca="false">($B$7/(G6*$B$13))*F6</f>
+        <v>96068.0834203608</v>
       </c>
       <c r="N6" s="20" t="n">
-        <f aca="false">M6/$B$7</f>
-        <v>57.3807488557283</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="25" t="n">
+        <f aca="false">M6/$B$8</f>
+        <v>40.1665241990099</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="26" t="n">
+        <f aca="false">B6*B5</f>
+        <v>6378.2887</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="N7" s="20"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="28" t="n">
         <f aca="false">B4*B3</f>
         <v>2391.745</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="0" t="s">
+      <c r="C8" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="27" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="E9" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <f aca="false">1.59*1.053</f>
         <v>1.67427</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G9" s="0" t="n">
         <v>0.34</v>
       </c>
-      <c r="H8" s="19" t="n">
-        <f aca="false">($B$10/F8)*G8</f>
+      <c r="H9" s="19" t="n">
+        <f aca="false">($B$11/F9)*G9</f>
         <v>242.850107808179</v>
       </c>
-      <c r="I8" s="20" t="n">
-        <f aca="false">H8/$B$5</f>
-        <v>0.0266521450284502</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <f aca="false">($B$5/G8)*F8</f>
-        <v>44869.6530325588</v>
-      </c>
-      <c r="K8" s="20" t="n">
-        <f aca="false">J8/$B$7</f>
-        <v>18.7602160901596</v>
-      </c>
-      <c r="L8" s="20" t="n">
-        <f aca="false">(H8*$B$12)/$B$5</f>
-        <v>0.00888404834281675</v>
-      </c>
-      <c r="M8" s="1" t="n">
-        <f aca="false">($B$5/(G8*$B$12))*F8</f>
-        <v>134608.959097676</v>
-      </c>
-      <c r="N8" s="20" t="n">
-        <f aca="false">M8/$B$7</f>
-        <v>56.2806482704788</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="28" t="n">
+      <c r="I9" s="20" t="n">
+        <f aca="false">H9/$B$7</f>
+        <v>0.0380744928977861</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <f aca="false">($B$7/G9)*F9</f>
+        <v>31408.7571227912</v>
+      </c>
+      <c r="K9" s="20" t="n">
+        <f aca="false">J9/$B$8</f>
+        <v>13.1321512631117</v>
+      </c>
+      <c r="L9" s="21" t="n">
+        <f aca="false">(H9*$B$13)/$B$7</f>
+        <v>0.0126914976325953</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <f aca="false">($B$7/(G9*$B$13))*F9</f>
+        <v>94226.2713683736</v>
+      </c>
+      <c r="N9" s="20" t="n">
+        <f aca="false">M9/$B$8</f>
+        <v>39.3964537893352</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="31" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="25" t="n">
-        <f aca="false">B9*B7</f>
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="28" t="n">
+        <f aca="false">B10*B8</f>
         <v>1195.8725</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="26" t="n">
+      <c r="C11" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">1.046*1.69</f>
+        <v>1.76774</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H11" s="19" t="n">
+        <f aca="false">($B$11/F11)*G11</f>
+        <v>270.599183137792</v>
+      </c>
+      <c r="I11" s="20" t="n">
+        <f aca="false">H11/$B$7</f>
+        <v>0.0424250446891486</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <f aca="false">($B$7/G11)*F11</f>
+        <v>28187.890166345</v>
+      </c>
+      <c r="K11" s="20" t="n">
+        <f aca="false">J11/$B$8</f>
+        <v>11.7854914158261</v>
+      </c>
+      <c r="L11" s="21" t="n">
+        <f aca="false">(H11*$B$13)/$B$7</f>
+        <v>0.0141416815630495</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <f aca="false">($B$7/(G11*$B$13))*F11</f>
+        <v>84563.6704990351</v>
+      </c>
+      <c r="N11" s="20" t="n">
+        <f aca="false">M11/$B$8</f>
+        <v>35.3564742474783</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="29" t="n">
         <f aca="false">1/3</f>
         <v>0.333333333333333</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="29" t="n">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="32" t="n">
         <v>0.00064516</v>
       </c>
     </row>

</xml_diff>